<commit_message>
Fixed major bug for 2015 causes of death
updated readme.md
added new_day.bat
</commit_message>
<xml_diff>
--- a/us_cause_of_death_2015_t.xlsx
+++ b/us_cause_of_death_2015_t.xlsx
@@ -345,8 +345,8 @@
   </sheetPr>
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -427,16 +427,16 @@
         <v>17</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>51909</v>
+        <v>12981</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1.05867920545523</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>12981</v>
+        <v>10354</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>0.264746282263467</v>
@@ -445,7 +445,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>10354</v>
+        <v>3279</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0.211168862688232</v>
@@ -454,7 +454,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>3279</v>
+        <v>2937</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>0.066874898662808</v>
@@ -463,7 +463,7 @@
         <v>21</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>2937</v>
+        <v>2552</v>
       </c>
       <c r="P2" s="0" t="n">
         <v>0.0598998406138051</v>
@@ -477,16 +477,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>4316</v>
+        <v>978</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.589984211497584</v>
+        <v>0.348850720051398</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>978</v>
+        <v>846</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>0.133689656822205</v>
@@ -495,7 +495,7 @@
         <v>21</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>846</v>
+        <v>388</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0.115645654060926</v>
@@ -504,7 +504,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>388</v>
+        <v>204</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>0.0530384323589116</v>
@@ -513,7 +513,7 @@
         <v>23</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="P3" s="0" t="n">
         <v>0.0278861860856133</v>
@@ -527,16 +527,16 @@
         <v>18</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>54299</v>
+        <v>11776</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.7459968563141</v>
+        <v>0.00276147568314581</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>11776</v>
+        <v>11458</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>0.161786754451368</v>
@@ -545,7 +545,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>11458</v>
+        <v>3681</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0.157417852624302</v>
@@ -554,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>3681</v>
+        <v>3539</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>0.0505720994510434</v>
@@ -563,7 +563,7 @@
         <v>25</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>3539</v>
+        <v>2943</v>
       </c>
       <c r="P4" s="0" t="n">
         <v>0.0486212061823533</v>
@@ -577,16 +577,16 @@
         <v>17</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>31617</v>
+        <v>7938</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>1.04768235445377</v>
+        <v>0.0975212439243901</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>7938</v>
+        <v>6727</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0.263038951502483</v>
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>6727</v>
+        <v>2270</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0.222910434209776</v>
@@ -604,7 +604,7 @@
         <v>20</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>2270</v>
+        <v>1653</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>0.0752202594999543</v>
@@ -613,7 +613,7 @@
         <v>21</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>1653</v>
+        <v>1538</v>
       </c>
       <c r="P5" s="0" t="n">
         <v>0.054774929054372</v>
@@ -627,16 +627,16 @@
         <v>17</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>259206</v>
+        <v>61289</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.656014722330353</v>
+        <v>0.00389246638945118</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>61289</v>
+        <v>59629</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0.155114026360906</v>
@@ -645,7 +645,7 @@
         <v>25</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>59629</v>
+        <v>15065</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0.150912794757207</v>
@@ -663,7 +663,7 @@
         <v>19</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>15065</v>
+        <v>13621</v>
       </c>
       <c r="P6" s="0" t="n">
         <v>0.0381274422347738</v>
@@ -677,16 +677,16 @@
         <v>18</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>36349</v>
+        <v>7604</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.631197540571403</v>
+        <v>0.236527599112027</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>7604</v>
+        <v>7009</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>0.132042864962033</v>
@@ -695,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>7009</v>
+        <v>2725</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0.121710736522737</v>
@@ -704,7 +704,7 @@
         <v>19</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>2725</v>
+        <v>2577</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>0.0473194117598028</v>
@@ -713,7 +713,7 @@
         <v>20</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>2577</v>
+        <v>1856</v>
       </c>
       <c r="P7" s="0" t="n">
         <v>0.0447494033412888</v>
@@ -727,16 +727,16 @@
         <v>17</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>30535</v>
+        <v>7205</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.856452790476615</v>
+        <v>0.0520575201940265</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>7205</v>
+        <v>6666</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>0.202087517779074</v>
@@ -745,7 +745,7 @@
         <v>21</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>6666</v>
+        <v>1799</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0.18696952026583</v>
@@ -754,7 +754,7 @@
         <v>20</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>1799</v>
+        <v>1388</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>0.0504587709208263</v>
@@ -763,7 +763,7 @@
         <v>19</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>1388</v>
+        <v>1369</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>0.0389309472140672</v>
@@ -777,16 +777,16 @@
         <v>18</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>8582</v>
+        <v>2010</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.88132237379899</v>
+        <v>0.140588479344071</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>2010</v>
+        <v>1940</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>0.206415517517591</v>
@@ -795,7 +795,7 @@
         <v>19</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>1940</v>
+        <v>510</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0.199226917405039</v>
@@ -804,7 +804,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>510</v>
+        <v>466</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>0.0523740865343143</v>
@@ -813,7 +813,7 @@
         <v>21</v>
       </c>
       <c r="O9" s="0" t="n">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="P9" s="0" t="n">
         <v>0.0478555378921381</v>
@@ -827,16 +827,16 @@
         <v>17</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>4871</v>
+        <v>1217</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.690188721485967</v>
+        <v>0.0636203522782179</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>1217</v>
+        <v>1072</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>0.172440910295303</v>
@@ -845,7 +845,7 @@
         <v>21</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>1072</v>
+        <v>265</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0.151895362232182</v>
@@ -854,7 +854,7 @@
         <v>20</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>0.0375487602532912</v>
@@ -863,7 +863,7 @@
         <v>32</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>242</v>
+        <v>162</v>
       </c>
       <c r="P10" s="0" t="n">
         <v>0.0342898112501753</v>
@@ -877,16 +877,16 @@
         <v>17</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>191737</v>
+        <v>45441</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.892724405741629</v>
+        <v>0.000754269409295774</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>45441</v>
+        <v>44027</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>0.211572569307465</v>
@@ -895,7 +895,7 @@
         <v>19</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>44027</v>
+        <v>11705</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0.204989007920155</v>
@@ -904,7 +904,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>11705</v>
+        <v>11433</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>0.0544982928136237</v>
@@ -913,7 +913,7 @@
         <v>21</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>11433</v>
+        <v>10578</v>
       </c>
       <c r="P11" s="0" t="n">
         <v>0.0532318651634481</v>
@@ -927,16 +927,16 @@
         <v>17</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>79942</v>
+        <v>17769</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0.752932232237521</v>
+        <v>0.0996286952116347</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>17769</v>
+        <v>16945</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>0.16735699425369</v>
@@ -945,7 +945,7 @@
         <v>19</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>16945</v>
+        <v>4607</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0.159596165660914</v>
@@ -954,7 +954,7 @@
         <v>21</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>4607</v>
+        <v>4344</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>0.0433909433579127</v>
@@ -963,7 +963,7 @@
         <v>20</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>4344</v>
+        <v>4335</v>
       </c>
       <c r="P12" s="0" t="n">
         <v>0.0409138827755097</v>
@@ -977,16 +977,16 @@
         <v>17</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>11053</v>
+        <v>2605</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.780649663246395</v>
+        <v>0.306171744338471</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>2605</v>
+        <v>2462</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>0.183985558016544</v>
@@ -995,7 +995,7 @@
         <v>20</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>2462</v>
+        <v>735</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0.173885774985309</v>
@@ -1004,7 +1004,7 @@
         <v>36</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>735</v>
+        <v>557</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>0.0519114722234778</v>
@@ -1013,7 +1013,7 @@
         <v>21</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>557</v>
+        <v>536</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>0.0393397143244587</v>
@@ -1027,16 +1027,16 @@
         <v>18</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>13026</v>
+        <v>2849</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0.72890465651781</v>
+        <v>0.0299933130580029</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>2849</v>
+        <v>2825</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>0.159423412131064</v>
@@ -1045,7 +1045,7 @@
         <v>19</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>2825</v>
+        <v>843</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0.158080427964288</v>
@@ -1054,7 +1054,7 @@
         <v>21</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>843</v>
+        <v>746</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>0.0471723188580158</v>
@@ -1063,7 +1063,7 @@
         <v>20</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>746</v>
+        <v>641</v>
       </c>
       <c r="P14" s="0" t="n">
         <v>0.0417444245172951</v>
@@ -1077,16 +1077,16 @@
         <v>17</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>106872</v>
+        <v>25652</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0.843383125440298</v>
+        <v>0.00505846791869929</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>25652</v>
+        <v>24713</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>0.202433415055342</v>
@@ -1095,7 +1095,7 @@
         <v>20</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>24713</v>
+        <v>5709</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0.195023272503613</v>
@@ -1104,7 +1104,7 @@
         <v>19</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>5709</v>
+        <v>5544</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>0.0450527197314419</v>
@@ -1113,7 +1113,7 @@
         <v>21</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>5544</v>
+        <v>4850</v>
       </c>
       <c r="P15" s="0" t="n">
         <v>0.0437506180050997</v>
@@ -1127,16 +1127,16 @@
         <v>17</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>62713</v>
+        <v>13948</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0.931535352608107</v>
+        <v>0.072041625502676</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>13948</v>
+        <v>13511</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>0.207182802579655</v>
@@ -1145,7 +1145,7 @@
         <v>19</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>13511</v>
+        <v>4212</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>0.200691629312712</v>
@@ -1154,7 +1154,7 @@
         <v>21</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>4212</v>
+        <v>3258</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>0.0625648096118085</v>
@@ -1163,7 +1163,7 @@
         <v>20</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>3258</v>
+        <v>2959</v>
       </c>
       <c r="P16" s="0" t="n">
         <v>0.0483941476057151</v>
@@ -1177,16 +1177,16 @@
         <v>17</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>29600</v>
+        <v>6813</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.93817252866022</v>
+        <v>0.0937855578481618</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>6813</v>
+        <v>6513</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>0.215938156681151</v>
@@ -1195,7 +1195,7 @@
         <v>19</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>6513</v>
+        <v>2011</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>0.206429651323109</v>
@@ -1204,7 +1204,7 @@
         <v>21</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>2011</v>
+        <v>1537</v>
       </c>
       <c r="M17" s="0" t="n">
         <v>0.0637386809167467</v>
@@ -1213,7 +1213,7 @@
         <v>20</v>
       </c>
       <c r="O17" s="0" t="n">
-        <v>1537</v>
+        <v>1418</v>
       </c>
       <c r="P17" s="0" t="n">
         <v>0.0487152424510391</v>
@@ -1227,16 +1227,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>26664</v>
+        <v>5624</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.915246348316728</v>
+        <v>0.0486730918809301</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>5624</v>
+        <v>5604</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>0.193044759335932</v>
@@ -1245,7 +1245,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>5604</v>
+        <v>1704</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>0.192358255924353</v>
@@ -1254,7 +1254,7 @@
         <v>21</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>1704</v>
+        <v>1475</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>0.0584900906665056</v>
@@ -1263,7 +1263,7 @@
         <v>20</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>1475</v>
+        <v>1364</v>
       </c>
       <c r="P18" s="0" t="n">
         <v>0.0506296266039294</v>
@@ -1277,16 +1277,16 @@
         <v>18</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>46564</v>
+        <v>10312</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>1.0422427961939</v>
+        <v>0.0305304349714046</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>10312</v>
+        <v>10077</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>0.230813669666513</v>
@@ -1295,7 +1295,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>10077</v>
+        <v>3331</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>0.22555366070883</v>
@@ -1304,7 +1304,7 @@
         <v>21</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>3331</v>
+        <v>2962</v>
       </c>
       <c r="M19" s="0" t="n">
         <v>0.0745578290980562</v>
@@ -1313,7 +1313,7 @@
         <v>20</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>2962</v>
+        <v>2050</v>
       </c>
       <c r="P19" s="0" t="n">
         <v>0.0662984958836513</v>
@@ -1327,16 +1327,16 @@
         <v>17</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>43716</v>
+        <v>10665</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0.940372922525713</v>
+        <v>0.0440974583945858</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>10665</v>
+        <v>9397</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>0.229414338428418</v>
@@ -1345,7 +1345,7 @@
         <v>21</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>9397</v>
+        <v>2578</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>0.202138447089718</v>
@@ -1354,7 +1354,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>2578</v>
+        <v>2280</v>
       </c>
       <c r="M20" s="0" t="n">
         <v>0.0554552428006059</v>
@@ -1363,7 +1363,7 @@
         <v>19</v>
       </c>
       <c r="O20" s="0" t="n">
-        <v>2280</v>
+        <v>2178</v>
       </c>
       <c r="P20" s="0" t="n">
         <v>0.0490449781169052</v>
@@ -1377,16 +1377,16 @@
         <v>18</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>14479</v>
+        <v>3398</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1.07713664213681</v>
+        <v>0.162028013438356</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>3398</v>
+        <v>3009</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>0.252787506732569</v>
@@ -1395,7 +1395,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>3009</v>
+        <v>1025</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>0.223848619116627</v>
@@ -1404,7 +1404,7 @@
         <v>21</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>1025</v>
+        <v>802</v>
       </c>
       <c r="M21" s="0" t="n">
         <v>0.0762528529725966</v>
@@ -1413,7 +1413,7 @@
         <v>20</v>
       </c>
       <c r="O21" s="0" t="n">
-        <v>802</v>
+        <v>616</v>
       </c>
       <c r="P21" s="0" t="n">
         <v>0.0596632078868512</v>
@@ -1427,16 +1427,16 @@
         <v>17</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>47247</v>
+        <v>11481</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0.781500178639954</v>
+        <v>0.0101890936999643</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>11481</v>
+        <v>10568</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0.189904196054042</v>
@@ -1445,7 +1445,7 @@
         <v>20</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>10568</v>
+        <v>2540</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>0.174802503605881</v>
@@ -1454,7 +1454,7 @@
         <v>19</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>2540</v>
+        <v>2040</v>
       </c>
       <c r="M22" s="0" t="n">
         <v>0.0420134707758267</v>
@@ -1463,7 +1463,7 @@
         <v>21</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>2040</v>
+        <v>1903</v>
       </c>
       <c r="P22" s="0" t="n">
         <v>0.0337431025128687</v>
@@ -1477,16 +1477,16 @@
         <v>18</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>57806</v>
+        <v>12750</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0.838679359298066</v>
+        <v>0.0276097086936342</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>12750</v>
+        <v>12130</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>0.184983597395605</v>
@@ -1495,7 +1495,7 @@
         <v>21</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>12130</v>
+        <v>3229</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>0.175988316581074</v>
@@ -1504,7 +1504,7 @@
         <v>19</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>3229</v>
+        <v>2784</v>
       </c>
       <c r="M23" s="0" t="n">
         <v>0.0468480028227772</v>
@@ -1513,7 +1513,7 @@
         <v>20</v>
       </c>
       <c r="O23" s="0" t="n">
-        <v>2784</v>
+        <v>2475</v>
       </c>
       <c r="P23" s="0" t="n">
         <v>0.0403917125607345</v>
@@ -1527,16 +1527,16 @@
         <v>17</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>95140</v>
+        <v>24794</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.952652070616411</v>
+        <v>0.02478257173403</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>24794</v>
+        <v>20732</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>0.24826629639335</v>
@@ -1545,7 +1545,7 @@
         <v>19</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>20732</v>
+        <v>5848</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>0.207592839268651</v>
@@ -1554,7 +1554,7 @@
         <v>20</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>5848</v>
+        <v>4666</v>
       </c>
       <c r="M24" s="0" t="n">
         <v>0.0585569614143869</v>
@@ -1563,7 +1563,7 @@
         <v>21</v>
       </c>
       <c r="O24" s="0" t="n">
-        <v>4666</v>
+        <v>4647</v>
       </c>
       <c r="P24" s="0" t="n">
         <v>0.046721405943832</v>
@@ -1577,16 +1577,16 @@
         <v>18</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>42800</v>
+        <v>9925</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>0.758914766069843</v>
+        <v>0.0823989934094991</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>9925</v>
+        <v>7844</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>0.175986660122504</v>
@@ -1595,7 +1595,7 @@
         <v>21</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>7844</v>
+        <v>2574</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>0.13908708937037</v>
@@ -1604,7 +1604,7 @@
         <v>19</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>2574</v>
+        <v>2351</v>
       </c>
       <c r="M25" s="0" t="n">
         <v>0.0456412758846677</v>
@@ -1613,7 +1613,7 @@
         <v>20</v>
       </c>
       <c r="O25" s="0" t="n">
-        <v>2351</v>
+        <v>2238</v>
       </c>
       <c r="P25" s="0" t="n">
         <v>0.0416871171736028</v>
@@ -1627,16 +1627,16 @@
         <v>17</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>31783</v>
+        <v>7969</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>1.06792368258444</v>
+        <v>0.0751978479572091</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>7969</v>
+        <v>6485</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>0.267762131533065</v>
@@ -1645,7 +1645,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>6485</v>
+        <v>1924</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>0.217899036640975</v>
@@ -1654,7 +1654,7 @@
         <v>21</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>1924</v>
+        <v>1814</v>
       </c>
       <c r="M26" s="0" t="n">
         <v>0.0646473009247857</v>
@@ -1663,7 +1663,7 @@
         <v>20</v>
       </c>
       <c r="O26" s="0" t="n">
-        <v>1814</v>
+        <v>1734</v>
       </c>
       <c r="P26" s="0" t="n">
         <v>0.0609512494166119</v>
@@ -1677,16 +1677,16 @@
         <v>17</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>59871</v>
+        <v>14808</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0.90352622876081</v>
+        <v>0.0261681695757753</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>14808</v>
+        <v>12965</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>0.223470735339147</v>
@@ -1695,7 +1695,7 @@
         <v>19</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>12965</v>
+        <v>3935</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>0.195657623154514</v>
@@ -1704,7 +1704,7 @@
         <v>21</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>3935</v>
+        <v>3309</v>
       </c>
       <c r="M27" s="0" t="n">
         <v>0.0593839373014279</v>
@@ -1713,7 +1713,7 @@
         <v>20</v>
       </c>
       <c r="O27" s="0" t="n">
-        <v>3309</v>
+        <v>3037</v>
       </c>
       <c r="P27" s="0" t="n">
         <v>0.0499368357129415</v>
@@ -1727,16 +1727,16 @@
         <v>18</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>9942</v>
+        <v>2130</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>0.930221243326491</v>
+        <v>0.284156298127394</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>2130</v>
+        <v>2104</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>0.199293024369888</v>
@@ -1745,7 +1745,7 @@
         <v>19</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>2104</v>
+        <v>679</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>0.196860339565373</v>
@@ -1754,7 +1754,7 @@
         <v>21</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>679</v>
+        <v>637</v>
       </c>
       <c r="M28" s="0" t="n">
         <v>0.0635304993179126</v>
@@ -1763,7 +1763,7 @@
         <v>20</v>
       </c>
       <c r="O28" s="0" t="n">
-        <v>637</v>
+        <v>458</v>
       </c>
       <c r="P28" s="0" t="n">
         <v>0.059600777710619</v>
@@ -1777,16 +1777,16 @@
         <v>17</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>16740</v>
+        <v>3591</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>0.86538103647214</v>
+        <v>0.0236764943073023</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>3591</v>
+        <v>3514</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>0.185638190081927</v>
@@ -1795,7 +1795,7 @@
         <v>19</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>3514</v>
+        <v>1174</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>0.181657644095765</v>
@@ -1804,7 +1804,7 @@
         <v>21</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>1174</v>
+        <v>799</v>
       </c>
       <c r="M29" s="0" t="n">
         <v>0.0606904024383687</v>
@@ -1813,7 +1813,7 @@
         <v>20</v>
       </c>
       <c r="O29" s="0" t="n">
-        <v>799</v>
+        <v>776</v>
       </c>
       <c r="P29" s="0" t="n">
         <v>0.0413046265317348</v>
@@ -1827,16 +1827,16 @@
         <v>17</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>22879</v>
+        <v>6114</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.742787053642738</v>
+        <v>0.0251935291589127</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>6114</v>
+        <v>5015</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>0.198496439790712</v>
@@ -1845,7 +1845,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="0" t="n">
-        <v>5015</v>
+        <v>1617</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>0.162816428778283</v>
@@ -1854,7 +1854,7 @@
         <v>21</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>1617</v>
+        <v>1340</v>
       </c>
       <c r="M30" s="0" t="n">
         <v>0.0524973410437653</v>
@@ -1863,7 +1863,7 @@
         <v>20</v>
       </c>
       <c r="O30" s="0" t="n">
-        <v>1340</v>
+        <v>1078</v>
       </c>
       <c r="P30" s="0" t="n">
         <v>0.0435042900424524</v>
@@ -1877,16 +1877,16 @@
         <v>18</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>11984</v>
+        <v>2773</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0.881363760387318</v>
+        <v>0.0792815532124106</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>2773</v>
+        <v>2571</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>0.203940396157713</v>
@@ -1895,7 +1895,7 @@
         <v>21</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>2571</v>
+        <v>815</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>0.189084298060397</v>
@@ -1904,7 +1904,7 @@
         <v>19</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>815</v>
+        <v>705</v>
       </c>
       <c r="M31" s="0" t="n">
         <v>0.0599392076698651</v>
@@ -1913,7 +1913,7 @@
         <v>20</v>
       </c>
       <c r="O31" s="0" t="n">
-        <v>705</v>
+        <v>457</v>
       </c>
       <c r="P31" s="0" t="n">
         <v>0.0518492532604355</v>
@@ -1927,16 +1927,16 @@
         <v>17</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>72271</v>
+        <v>18647</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0.813661945984042</v>
+        <v>0.00514512749670971</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>18647</v>
+        <v>16270</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>0.209936963744302</v>
@@ -1945,7 +1945,7 @@
         <v>20</v>
       </c>
       <c r="I32" s="0" t="n">
-        <v>16270</v>
+        <v>3413</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>0.183175545670606</v>
@@ -1954,7 +1954,7 @@
         <v>21</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>3413</v>
+        <v>3218</v>
       </c>
       <c r="M32" s="0" t="n">
         <v>0.0384252081975279</v>
@@ -1963,7 +1963,7 @@
         <v>19</v>
       </c>
       <c r="O32" s="0" t="n">
-        <v>3218</v>
+        <v>3202</v>
       </c>
       <c r="P32" s="0" t="n">
         <v>0.0362298036858027</v>
@@ -1977,16 +1977,16 @@
         <v>18</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>17685</v>
+        <v>3591</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0.843416415930913</v>
+        <v>0.152706777710533</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>3591</v>
+        <v>3508</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>0.171258600486735</v>
@@ -1995,7 +1995,7 @@
         <v>21</v>
       </c>
       <c r="I33" s="0" t="n">
-        <v>3508</v>
+        <v>1430</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>0.167300242413664</v>
@@ -2004,7 +2004,7 @@
         <v>19</v>
       </c>
       <c r="L33" s="0" t="n">
-        <v>1430</v>
+        <v>1109</v>
       </c>
       <c r="M33" s="0" t="n">
         <v>0.0681982174035174</v>
@@ -2013,7 +2013,7 @@
         <v>20</v>
       </c>
       <c r="O33" s="0" t="n">
-        <v>1109</v>
+        <v>786</v>
       </c>
       <c r="P33" s="0" t="n">
         <v>0.052889386783567</v>
@@ -2027,16 +2027,16 @@
         <v>17</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>153628</v>
+        <v>44450</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>0.789716597388005</v>
+        <v>0.00404039137101942</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>44450</v>
+        <v>35089</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>0.228492870791111</v>
@@ -2045,7 +2045,7 @@
         <v>19</v>
       </c>
       <c r="I34" s="0" t="n">
-        <v>35089</v>
+        <v>7109</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>0.180373146078499</v>
@@ -2054,7 +2054,7 @@
         <v>21</v>
       </c>
       <c r="L34" s="0" t="n">
-        <v>7109</v>
+        <v>6515</v>
       </c>
       <c r="M34" s="0" t="n">
         <v>0.036543437985467</v>
@@ -2063,7 +2063,7 @@
         <v>20</v>
       </c>
       <c r="O34" s="0" t="n">
-        <v>6515</v>
+        <v>6292</v>
       </c>
       <c r="P34" s="0" t="n">
         <v>0.0334900124455363</v>
@@ -2077,16 +2077,16 @@
         <v>18</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>89133</v>
+        <v>19322</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>0.849850172824703</v>
+        <v>0.0599918917506763</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>19322</v>
+        <v>18474</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>0.184228120217191</v>
@@ -2095,7 +2095,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>18474</v>
+        <v>5221</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>0.176142754005403</v>
@@ -2104,7 +2104,7 @@
         <v>20</v>
       </c>
       <c r="L35" s="0" t="n">
-        <v>5221</v>
+        <v>5033</v>
       </c>
       <c r="M35" s="0" t="n">
         <v>0.0497803030563066</v>
@@ -2113,7 +2113,7 @@
         <v>21</v>
       </c>
       <c r="O35" s="0" t="n">
-        <v>5033</v>
+        <v>4991</v>
       </c>
       <c r="P35" s="0" t="n">
         <v>0.047987792622561</v>
@@ -2127,16 +2127,16 @@
         <v>17</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>6223</v>
+        <v>1323</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>0.816600224128745</v>
+        <v>0.65493358808076</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>1323</v>
+        <v>1320</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>0.173607921665166</v>
@@ -2145,7 +2145,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>1320</v>
+        <v>376</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>0.173214252908556</v>
@@ -2154,7 +2154,7 @@
         <v>21</v>
       </c>
       <c r="L36" s="0" t="n">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="M36" s="0" t="n">
         <v>0.0493398174951644</v>
@@ -2163,7 +2163,7 @@
         <v>19</v>
       </c>
       <c r="O36" s="0" t="n">
-        <v>368</v>
+        <v>351</v>
       </c>
       <c r="P36" s="0" t="n">
         <v>0.0482900341442035</v>
@@ -2177,16 +2177,16 @@
         <v>17</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>118188</v>
+        <v>28069</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>1.011095807205</v>
+        <v>0.00300279747799232</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>28069</v>
+        <v>25396</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>0.240129693475118</v>
@@ -2195,7 +2195,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="0" t="n">
-        <v>25396</v>
+        <v>7211</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>0.217262235758099</v>
@@ -2204,7 +2204,7 @@
         <v>21</v>
       </c>
       <c r="L37" s="0" t="n">
-        <v>7211</v>
+        <v>6756</v>
       </c>
       <c r="M37" s="0" t="n">
         <v>0.0616899504666741</v>
@@ -2213,7 +2213,7 @@
         <v>20</v>
       </c>
       <c r="O37" s="0" t="n">
-        <v>6756</v>
+        <v>5945</v>
       </c>
       <c r="P37" s="0" t="n">
         <v>0.0577974352174248</v>
@@ -2227,16 +2227,16 @@
         <v>17</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>39422</v>
+        <v>10310</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0.996267094199073</v>
+        <v>0.150241181954581</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>10310</v>
+        <v>8280</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>0.26055283195151</v>
@@ -2245,7 +2245,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>8280</v>
+        <v>2924</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>0.209250964942629</v>
@@ -2254,7 +2254,7 @@
         <v>21</v>
       </c>
       <c r="L38" s="0" t="n">
-        <v>2924</v>
+        <v>2422</v>
       </c>
       <c r="M38" s="0" t="n">
         <v>0.0738949059773246</v>
@@ -2263,7 +2263,7 @@
         <v>20</v>
       </c>
       <c r="O38" s="0" t="n">
-        <v>2422</v>
+        <v>1881</v>
       </c>
       <c r="P38" s="0" t="n">
         <v>0.061208434431286</v>
@@ -2277,16 +2277,16 @@
         <v>18</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>35705</v>
+        <v>8093</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.846544011634675</v>
+        <v>0.0445973753223589</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>8093</v>
+        <v>6859</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>0.191880148050957</v>
@@ -2295,7 +2295,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>6859</v>
+        <v>2119</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>0.162622752438097</v>
@@ -2304,7 +2304,7 @@
         <v>21</v>
       </c>
       <c r="L39" s="0" t="n">
-        <v>2119</v>
+        <v>1999</v>
       </c>
       <c r="M39" s="0" t="n">
         <v>0.0502402117533644</v>
@@ -2313,7 +2313,7 @@
         <v>20</v>
       </c>
       <c r="O39" s="0" t="n">
-        <v>1999</v>
+        <v>1873</v>
       </c>
       <c r="P39" s="0" t="n">
         <v>0.0473950841410927</v>
@@ -2327,16 +2327,16 @@
         <v>17</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>132598</v>
+        <v>32042</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>1.03576092746213</v>
+        <v>0.0146305390513927</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>32042</v>
+        <v>28697</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>0.250289232399747</v>
@@ -2345,7 +2345,7 @@
         <v>21</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>28697</v>
+        <v>7324</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>0.224160480062903</v>
@@ -2354,7 +2354,7 @@
         <v>20</v>
       </c>
       <c r="L40" s="0" t="n">
-        <v>7324</v>
+        <v>6987</v>
       </c>
       <c r="M40" s="0" t="n">
         <v>0.0572098601240792</v>
@@ -2363,7 +2363,7 @@
         <v>19</v>
       </c>
       <c r="O40" s="0" t="n">
-        <v>6987</v>
+        <v>6664</v>
       </c>
       <c r="P40" s="0" t="n">
         <v>0.0545774566748964</v>
@@ -2377,16 +2377,16 @@
         <v>17</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>10163</v>
+        <v>2371</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>0.959351911199298</v>
+        <v>0.629058460713581</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>2371</v>
+        <v>2226</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>0.223814167219673</v>
@@ -2395,7 +2395,7 @@
         <v>21</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>2226</v>
+        <v>649</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>0.210126670700545</v>
@@ -2404,7 +2404,7 @@
         <v>19</v>
       </c>
       <c r="L41" s="0" t="n">
-        <v>649</v>
+        <v>510</v>
       </c>
       <c r="M41" s="0" t="n">
         <v>0.0612633464890627</v>
@@ -2413,7 +2413,7 @@
         <v>25</v>
       </c>
       <c r="O41" s="0" t="n">
-        <v>510</v>
+        <v>453</v>
       </c>
       <c r="P41" s="0" t="n">
         <v>0.0481422291362435</v>
@@ -2427,16 +2427,16 @@
         <v>17</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>47198</v>
+        <v>10092</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>0.916694926150491</v>
+        <v>0.00879831352061894</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>10092</v>
+        <v>9950</v>
       </c>
       <c r="G42" s="0" t="n">
         <v>0.196010110485842</v>
@@ -2445,7 +2445,7 @@
         <v>19</v>
       </c>
       <c r="I42" s="0" t="n">
-        <v>9950</v>
+        <v>2908</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>0.193252140243175</v>
@@ -2454,7 +2454,7 @@
         <v>21</v>
       </c>
       <c r="L42" s="0" t="n">
-        <v>2908</v>
+        <v>2737</v>
       </c>
       <c r="M42" s="0" t="n">
         <v>0.0564801229977039</v>
@@ -2463,7 +2463,7 @@
         <v>20</v>
       </c>
       <c r="O42" s="0" t="n">
-        <v>2737</v>
+        <v>2600</v>
       </c>
       <c r="P42" s="0" t="n">
         <v>0.0531589053111126</v>
@@ -2477,16 +2477,16 @@
         <v>17</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>7731</v>
+        <v>1711</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>0.873896043560287</v>
+        <v>0.293898553001778</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>1711</v>
+        <v>1640</v>
       </c>
       <c r="G43" s="0" t="n">
         <v>0.19340785545617</v>
@@ -2495,7 +2495,7 @@
         <v>19</v>
       </c>
       <c r="I43" s="0" t="n">
-        <v>1640</v>
+        <v>502</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>0.185382164201122</v>
@@ -2504,7 +2504,7 @@
         <v>21</v>
       </c>
       <c r="L43" s="0" t="n">
-        <v>502</v>
+        <v>469</v>
       </c>
       <c r="M43" s="0" t="n">
         <v>0.0567450283103433</v>
@@ -2513,7 +2513,7 @@
         <v>25</v>
       </c>
       <c r="O43" s="0" t="n">
-        <v>469</v>
+        <v>421</v>
       </c>
       <c r="P43" s="0" t="n">
         <v>0.0530147774453207</v>
@@ -2527,16 +2527,16 @@
         <v>17</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>66570</v>
+        <v>15730</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>0.97478845904351</v>
+        <v>0.00616472797442268</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>15730</v>
+        <v>14214</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>0.230335323129854</v>
@@ -2545,7 +2545,7 @@
         <v>19</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>14214</v>
+        <v>4239</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>0.208136445198204</v>
@@ -2554,7 +2554,7 @@
         <v>21</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>4239</v>
+        <v>3873</v>
       </c>
       <c r="M44" s="0" t="n">
         <v>0.0620719284645552</v>
@@ -2563,7 +2563,7 @@
         <v>20</v>
       </c>
       <c r="O44" s="0" t="n">
-        <v>3873</v>
+        <v>3447</v>
       </c>
       <c r="P44" s="0" t="n">
         <v>0.0567125687528243</v>
@@ -2577,16 +2577,16 @@
         <v>17</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>189654</v>
+        <v>43298</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>0.654072211153026</v>
+        <v>0.0118878953876242</v>
       </c>
       <c r="E45" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>43298</v>
+        <v>39121</v>
       </c>
       <c r="G45" s="0" t="n">
         <v>0.149324657526357</v>
@@ -2595,7 +2595,7 @@
         <v>20</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>39121</v>
+        <v>10485</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>0.134919163173556</v>
@@ -2604,7 +2604,7 @@
         <v>19</v>
       </c>
       <c r="L45" s="0" t="n">
-        <v>10485</v>
+        <v>10231</v>
       </c>
       <c r="M45" s="0" t="n">
         <v>0.0361603084244966</v>
@@ -2613,7 +2613,7 @@
         <v>21</v>
       </c>
       <c r="O45" s="0" t="n">
-        <v>10231</v>
+        <v>9976</v>
       </c>
       <c r="P45" s="0" t="n">
         <v>0.0352843219352431</v>
@@ -2627,16 +2627,16 @@
         <v>17</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>17334</v>
+        <v>3598</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>0.540680819898452</v>
+        <v>0.311170639166202</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>3598</v>
+        <v>3091</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>0.112228544478749</v>
@@ -2645,7 +2645,7 @@
         <v>21</v>
       </c>
       <c r="I46" s="0" t="n">
-        <v>3091</v>
+        <v>1223</v>
       </c>
       <c r="J46" s="0" t="n">
         <v>0.0964142387392474</v>
@@ -2654,7 +2654,7 @@
         <v>25</v>
       </c>
       <c r="L46" s="0" t="n">
-        <v>1223</v>
+        <v>906</v>
       </c>
       <c r="M46" s="0" t="n">
         <v>0.0381477237069232</v>
@@ -2663,7 +2663,7 @@
         <v>20</v>
       </c>
       <c r="O46" s="0" t="n">
-        <v>906</v>
+        <v>888</v>
       </c>
       <c r="P46" s="0" t="n">
         <v>0.0282598836291679</v>
@@ -2677,16 +2677,16 @@
         <v>18</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>5919</v>
+        <v>1399</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>0.948574413972041</v>
+        <v>0.142310200981107</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>1399</v>
+        <v>1311</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>0.224202670239379</v>
@@ -2695,7 +2695,7 @@
         <v>19</v>
       </c>
       <c r="I47" s="0" t="n">
-        <v>1311</v>
+        <v>357</v>
       </c>
       <c r="J47" s="0" t="n">
         <v>0.21009985752954</v>
@@ -2704,7 +2704,7 @@
         <v>21</v>
       </c>
       <c r="L47" s="0" t="n">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="M47" s="0" t="n">
         <v>0.0572125470160532</v>
@@ -2713,7 +2713,7 @@
         <v>20</v>
       </c>
       <c r="O47" s="0" t="n">
-        <v>346</v>
+        <v>307</v>
       </c>
       <c r="P47" s="0" t="n">
         <v>0.0554496954273232</v>
@@ -2727,16 +2727,16 @@
         <v>18</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>65577</v>
+        <v>14947</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>0.768283686088684</v>
+        <v>0.00359673500814655</v>
       </c>
       <c r="E48" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>14947</v>
+        <v>14077</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>0.175115303474809</v>
@@ -2745,7 +2745,7 @@
         <v>21</v>
       </c>
       <c r="I48" s="0" t="n">
-        <v>14077</v>
+        <v>3429</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>0.164922601660192</v>
@@ -2754,7 +2754,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="0" t="n">
-        <v>3429</v>
+        <v>3393</v>
       </c>
       <c r="M48" s="0" t="n">
         <v>0.0401733040486466</v>
@@ -2763,7 +2763,7 @@
         <v>19</v>
       </c>
       <c r="O48" s="0" t="n">
-        <v>3393</v>
+        <v>3370</v>
       </c>
       <c r="P48" s="0" t="n">
         <v>0.0397515370770073</v>
@@ -2777,16 +2777,16 @@
         <v>18</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>54595</v>
+        <v>12687</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>0.716950323530482</v>
+        <v>0.0442553821833084</v>
       </c>
       <c r="E49" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>12687</v>
+        <v>11025</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>0.166607725151227</v>
@@ -2795,7 +2795,7 @@
         <v>25</v>
       </c>
       <c r="I49" s="0" t="n">
-        <v>11025</v>
+        <v>3490</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>0.144782073759933</v>
@@ -2804,7 +2804,7 @@
         <v>21</v>
       </c>
       <c r="L49" s="0" t="n">
-        <v>3490</v>
+        <v>3192</v>
       </c>
       <c r="M49" s="0" t="n">
         <v>0.045831241489539</v>
@@ -2813,7 +2813,7 @@
         <v>19</v>
       </c>
       <c r="O49" s="0" t="n">
-        <v>3192</v>
+        <v>3154</v>
       </c>
       <c r="P49" s="0" t="n">
         <v>0.0419178575457331</v>
@@ -2827,16 +2827,16 @@
         <v>18</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>22752</v>
+        <v>4839</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>1.26953871529512</v>
+        <v>0.175990027603762</v>
       </c>
       <c r="E50" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>4839</v>
+        <v>4727</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>0.270011332775715</v>
@@ -2845,7 +2845,7 @@
         <v>19</v>
       </c>
       <c r="I50" s="0" t="n">
-        <v>4727</v>
+        <v>1628</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>0.263761845428974</v>
@@ -2854,7 +2854,7 @@
         <v>21</v>
       </c>
       <c r="L50" s="0" t="n">
-        <v>1628</v>
+        <v>1516</v>
       </c>
       <c r="M50" s="0" t="n">
         <v>0.0908407625044151</v>
@@ -2863,7 +2863,7 @@
         <v>20</v>
       </c>
       <c r="O50" s="0" t="n">
-        <v>1516</v>
+        <v>1079</v>
       </c>
       <c r="P50" s="0" t="n">
         <v>0.084591275157674</v>
@@ -2877,16 +2877,16 @@
         <v>17</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>51264</v>
+        <v>11473</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>0.880456523852396</v>
+        <v>0.0185317686726891</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>11473</v>
+        <v>11423</v>
       </c>
       <c r="G51" s="0" t="n">
         <v>0.197048176072069</v>
@@ -2895,7 +2895,7 @@
         <v>21</v>
       </c>
       <c r="I51" s="0" t="n">
-        <v>11423</v>
+        <v>3206</v>
       </c>
       <c r="J51" s="0" t="n">
         <v>0.196189428682232</v>
@@ -2904,7 +2904,7 @@
         <v>19</v>
       </c>
       <c r="L51" s="0" t="n">
-        <v>3206</v>
+        <v>2846</v>
       </c>
       <c r="M51" s="0" t="n">
         <v>0.0550628826363682</v>
@@ -2913,7 +2913,7 @@
         <v>20</v>
       </c>
       <c r="O51" s="0" t="n">
-        <v>2846</v>
+        <v>2618</v>
       </c>
       <c r="P51" s="0" t="n">
         <v>0.0488799014295396</v>
@@ -2927,16 +2927,16 @@
         <v>17</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>4778</v>
+        <v>1030</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0.825559516137114</v>
+        <v>0.452347177322512</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>1030</v>
+        <v>931</v>
       </c>
       <c r="G52" s="0" t="n">
         <v>0.177966994897704</v>
@@ -2945,7 +2945,7 @@
         <v>21</v>
       </c>
       <c r="I52" s="0" t="n">
-        <v>931</v>
+        <v>400</v>
       </c>
       <c r="J52" s="0" t="n">
         <v>0.160861429368701</v>
@@ -2954,7 +2954,7 @@
         <v>19</v>
       </c>
       <c r="L52" s="0" t="n">
-        <v>400</v>
+        <v>368</v>
       </c>
       <c r="M52" s="0" t="n">
         <v>0.0691133960767781</v>
@@ -2963,7 +2963,7 @@
         <v>20</v>
       </c>
       <c r="O52" s="0" t="n">
-        <v>368</v>
+        <v>198</v>
       </c>
       <c r="P52" s="0" t="n">
         <v>0.0635843243906358</v>

</xml_diff>

<commit_message>
Fixed 2015 cause of death per capita
</commit_message>
<xml_diff>
--- a/us_cause_of_death_2015_t.xlsx
+++ b/us_cause_of_death_2015_t.xlsx
@@ -345,8 +345,8 @@
   </sheetPr>
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -430,7 +430,7 @@
         <v>12981</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>0.264746282263467</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>18</v>
@@ -439,7 +439,7 @@
         <v>10354</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0.264746282263467</v>
+        <v>0.211168862688232</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>19</v>
@@ -448,7 +448,7 @@
         <v>3279</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>0.211168862688232</v>
+        <v>0.066874898662808</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>20</v>
@@ -457,7 +457,7 @@
         <v>2937</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>0.066874898662808</v>
+        <v>0.0598998406138051</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>21</v>
@@ -466,7 +466,7 @@
         <v>2552</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>0.0598998406138051</v>
+        <v>0.0520478015820329</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,7 +480,7 @@
         <v>978</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.348850720051398</v>
+        <v>0.133689656822205</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>17</v>
@@ -489,7 +489,7 @@
         <v>846</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0.133689656822205</v>
+        <v>0.115645654060926</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>21</v>
@@ -498,7 +498,7 @@
         <v>388</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>0.115645654060926</v>
+        <v>0.0530384323589116</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>19</v>
@@ -507,7 +507,7 @@
         <v>204</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>0.0530384323589116</v>
+        <v>0.0278861860856133</v>
       </c>
       <c r="N3" s="0" t="s">
         <v>23</v>
@@ -516,7 +516,7 @@
         <v>201</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>0.0278861860856133</v>
+        <v>0.0274760951137661</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,7 +530,7 @@
         <v>11776</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.00276147568314581</v>
+        <v>0.161786754451368</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>17</v>
@@ -539,7 +539,7 @@
         <v>11458</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.161786754451368</v>
+        <v>0.157417852624302</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>19</v>
@@ -548,7 +548,7 @@
         <v>3681</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0.157417852624302</v>
+        <v>0.0505720994510434</v>
       </c>
       <c r="K4" s="0" t="s">
         <v>21</v>
@@ -557,7 +557,7 @@
         <v>3539</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>0.0505720994510434</v>
+        <v>0.0486212061823533</v>
       </c>
       <c r="N4" s="0" t="s">
         <v>25</v>
@@ -566,7 +566,7 @@
         <v>2943</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>0.0486212061823533</v>
+        <v>0.0404329499278513</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,7 +580,7 @@
         <v>7938</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.0975212439243901</v>
+        <v>0.263038951502483</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>18</v>
@@ -589,7 +589,7 @@
         <v>6727</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.263038951502483</v>
+        <v>0.222910434209776</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>19</v>
@@ -598,7 +598,7 @@
         <v>2270</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0.222910434209776</v>
+        <v>0.0752202594999543</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>20</v>
@@ -607,7 +607,7 @@
         <v>1653</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>0.0752202594999543</v>
+        <v>0.054774929054372</v>
       </c>
       <c r="N5" s="0" t="s">
         <v>21</v>
@@ -616,7 +616,7 @@
         <v>1538</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>0.054774929054372</v>
+        <v>0.0509642110620836</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,7 +630,7 @@
         <v>61289</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.00389246638945118</v>
+        <v>0.155114026360906</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>18</v>
@@ -639,7 +639,7 @@
         <v>59629</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.155114026360906</v>
+        <v>0.150912794757207</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>25</v>
@@ -648,7 +648,7 @@
         <v>15065</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0.150912794757207</v>
+        <v>0.0381274422347738</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>20</v>
@@ -666,7 +666,7 @@
         <v>13621</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>0.0381274422347738</v>
+        <v>0.0344728769120381</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,7 +680,7 @@
         <v>7604</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.236527599112027</v>
+        <v>0.132042864962033</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>17</v>
@@ -689,7 +689,7 @@
         <v>7009</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.132042864962033</v>
+        <v>0.121710736522737</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>21</v>
@@ -698,7 +698,7 @@
         <v>2725</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0.121710736522737</v>
+        <v>0.0473194117598028</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>19</v>
@@ -707,7 +707,7 @@
         <v>2577</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>0.0473194117598028</v>
+        <v>0.0447494033412888</v>
       </c>
       <c r="N7" s="0" t="s">
         <v>20</v>
@@ -716,7 +716,7 @@
         <v>1856</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>0.0447494033412888</v>
+        <v>0.0322292947619061</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -730,7 +730,7 @@
         <v>7205</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.0520575201940265</v>
+        <v>0.202087517779074</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>18</v>
@@ -739,7 +739,7 @@
         <v>6666</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>0.202087517779074</v>
+        <v>0.18696952026583</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>21</v>
@@ -748,7 +748,7 @@
         <v>1799</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0.18696952026583</v>
+        <v>0.0504587709208263</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>20</v>
@@ -757,7 +757,7 @@
         <v>1388</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>0.0504587709208263</v>
+        <v>0.0389309472140672</v>
       </c>
       <c r="N8" s="0" t="s">
         <v>19</v>
@@ -766,7 +766,7 @@
         <v>1369</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>0.0389309472140672</v>
+        <v>0.0383980307896671</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -780,7 +780,7 @@
         <v>2010</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.140588479344071</v>
+        <v>0.206415517517591</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>17</v>
@@ -789,7 +789,7 @@
         <v>1940</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0.206415517517591</v>
+        <v>0.199226917405039</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>19</v>
@@ -798,7 +798,7 @@
         <v>510</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>0.199226917405039</v>
+        <v>0.0523740865343143</v>
       </c>
       <c r="K9" s="0" t="s">
         <v>20</v>
@@ -807,7 +807,7 @@
         <v>466</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>0.0523740865343143</v>
+        <v>0.0478555378921381</v>
       </c>
       <c r="N9" s="0" t="s">
         <v>21</v>
@@ -816,7 +816,7 @@
         <v>449</v>
       </c>
       <c r="P9" s="0" t="n">
-        <v>0.0478555378921381</v>
+        <v>0.046109735007661</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +830,7 @@
         <v>1217</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.0636203522782179</v>
+        <v>0.172440910295303</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>18</v>
@@ -839,7 +839,7 @@
         <v>1072</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0.172440910295303</v>
+        <v>0.151895362232182</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>21</v>
@@ -848,7 +848,7 @@
         <v>265</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0.151895362232182</v>
+        <v>0.0375487602532912</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>20</v>
@@ -857,7 +857,7 @@
         <v>242</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>0.0375487602532912</v>
+        <v>0.0342898112501753</v>
       </c>
       <c r="N10" s="0" t="s">
         <v>32</v>
@@ -866,7 +866,7 @@
         <v>162</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>0.0342898112501753</v>
+        <v>0.0229543364567289</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,7 +880,7 @@
         <v>45441</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.000754269409295774</v>
+        <v>0.211572569307465</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>18</v>
@@ -889,7 +889,7 @@
         <v>44027</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0.211572569307465</v>
+        <v>0.204989007920155</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>19</v>
@@ -898,7 +898,7 @@
         <v>11705</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0.204989007920155</v>
+        <v>0.0544982928136237</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>20</v>
@@ -907,7 +907,7 @@
         <v>11433</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>0.0544982928136237</v>
+        <v>0.0532318651634481</v>
       </c>
       <c r="N11" s="0" t="s">
         <v>21</v>
@@ -916,7 +916,7 @@
         <v>10578</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>0.0532318651634481</v>
+        <v>0.0492509988366093</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,7 +930,7 @@
         <v>17769</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0.0996286952116347</v>
+        <v>0.16735699425369</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>18</v>
@@ -939,7 +939,7 @@
         <v>16945</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.16735699425369</v>
+        <v>0.159596165660914</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>19</v>
@@ -948,7 +948,7 @@
         <v>4607</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0.159596165660914</v>
+        <v>0.0433909433579127</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>21</v>
@@ -957,7 +957,7 @@
         <v>4344</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>0.0433909433579127</v>
+        <v>0.0409138827755097</v>
       </c>
       <c r="N12" s="0" t="s">
         <v>20</v>
@@ -966,7 +966,7 @@
         <v>4335</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>0.0409138827755097</v>
+        <v>0.0408291164437924</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,7 +980,7 @@
         <v>2605</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.306171744338471</v>
+        <v>0.183985558016544</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>18</v>
@@ -989,7 +989,7 @@
         <v>2462</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.183985558016544</v>
+        <v>0.173885774985309</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>20</v>
@@ -998,7 +998,7 @@
         <v>735</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0.173885774985309</v>
+        <v>0.0519114722234778</v>
       </c>
       <c r="K13" s="0" t="s">
         <v>36</v>
@@ -1007,7 +1007,7 @@
         <v>557</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>0.0519114722234778</v>
+        <v>0.0393397143244587</v>
       </c>
       <c r="N13" s="0" t="s">
         <v>21</v>
@@ -1016,7 +1016,7 @@
         <v>536</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>0.0393397143244587</v>
+        <v>0.0378565294037879</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,7 +1030,7 @@
         <v>2849</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0.0299933130580029</v>
+        <v>0.159423412131064</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>17</v>
@@ -1039,7 +1039,7 @@
         <v>2825</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0.159423412131064</v>
+        <v>0.158080427964288</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>19</v>
@@ -1048,7 +1048,7 @@
         <v>843</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0.158080427964288</v>
+        <v>0.0471723188580158</v>
       </c>
       <c r="K14" s="0" t="s">
         <v>21</v>
@@ -1057,7 +1057,7 @@
         <v>746</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>0.0471723188580158</v>
+        <v>0.0417444245172951</v>
       </c>
       <c r="N14" s="0" t="s">
         <v>20</v>
@@ -1066,7 +1066,7 @@
         <v>641</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>0.0417444245172951</v>
+        <v>0.035868868787649</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,7 +1080,7 @@
         <v>25652</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0.00505846791869929</v>
+        <v>0.202433415055342</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>18</v>
@@ -1089,7 +1089,7 @@
         <v>24713</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0.202433415055342</v>
+        <v>0.195023272503613</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>20</v>
@@ -1098,7 +1098,7 @@
         <v>5709</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>0.195023272503613</v>
+        <v>0.0450527197314419</v>
       </c>
       <c r="K15" s="0" t="s">
         <v>19</v>
@@ -1107,7 +1107,7 @@
         <v>5544</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>0.0450527197314419</v>
+        <v>0.0437506180050997</v>
       </c>
       <c r="N15" s="0" t="s">
         <v>21</v>
@@ -1116,7 +1116,7 @@
         <v>4850</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>0.0437506180050997</v>
+        <v>0.038273899228848</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,7 +1130,7 @@
         <v>13948</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0.072041625502676</v>
+        <v>0.207182802579655</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>18</v>
@@ -1139,7 +1139,7 @@
         <v>13511</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>0.207182802579655</v>
+        <v>0.200691629312712</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>19</v>
@@ -1148,7 +1148,7 @@
         <v>4212</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0.200691629312712</v>
+        <v>0.0625648096118085</v>
       </c>
       <c r="K16" s="0" t="s">
         <v>21</v>
@@ -1157,7 +1157,7 @@
         <v>3258</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>0.0625648096118085</v>
+        <v>0.0483941476057151</v>
       </c>
       <c r="N16" s="0" t="s">
         <v>20</v>
@@ -1166,7 +1166,7 @@
         <v>2959</v>
       </c>
       <c r="P16" s="0" t="n">
-        <v>0.0483941476057151</v>
+        <v>0.0439528185283337</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1180,7 +1180,7 @@
         <v>6813</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.0937855578481618</v>
+        <v>0.215938156681151</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>18</v>
@@ -1189,7 +1189,7 @@
         <v>6513</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0.215938156681151</v>
+        <v>0.206429651323109</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>19</v>
@@ -1198,7 +1198,7 @@
         <v>2011</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0.206429651323109</v>
+        <v>0.0637386809167467</v>
       </c>
       <c r="K17" s="0" t="s">
         <v>21</v>
@@ -1207,7 +1207,7 @@
         <v>1537</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>0.0637386809167467</v>
+        <v>0.0487152424510391</v>
       </c>
       <c r="N17" s="0" t="s">
         <v>20</v>
@@ -1216,7 +1216,7 @@
         <v>1418</v>
       </c>
       <c r="P17" s="0" t="n">
-        <v>0.0487152424510391</v>
+        <v>0.0449435353256822</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,7 +1230,7 @@
         <v>5624</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.0486730918809301</v>
+        <v>0.193044759335932</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>18</v>
@@ -1239,7 +1239,7 @@
         <v>5604</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0.193044759335932</v>
+        <v>0.192358255924353</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>19</v>
@@ -1248,7 +1248,7 @@
         <v>1704</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0.192358255924353</v>
+        <v>0.0584900906665056</v>
       </c>
       <c r="K18" s="0" t="s">
         <v>21</v>
@@ -1257,7 +1257,7 @@
         <v>1475</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>0.0584900906665056</v>
+        <v>0.0506296266039294</v>
       </c>
       <c r="N18" s="0" t="s">
         <v>20</v>
@@ -1266,7 +1266,7 @@
         <v>1364</v>
       </c>
       <c r="P18" s="0" t="n">
-        <v>0.0506296266039294</v>
+        <v>0.0468195326696676</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,7 +1280,7 @@
         <v>10312</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0.0305304349714046</v>
+        <v>0.230813669666513</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>17</v>
@@ -1289,7 +1289,7 @@
         <v>10077</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>0.230813669666513</v>
+        <v>0.22555366070883</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>19</v>
@@ -1298,7 +1298,7 @@
         <v>3331</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0.22555366070883</v>
+        <v>0.0745578290980562</v>
       </c>
       <c r="K19" s="0" t="s">
         <v>21</v>
@@ -1307,7 +1307,7 @@
         <v>2962</v>
       </c>
       <c r="M19" s="0" t="n">
-        <v>0.0745578290980562</v>
+        <v>0.0662984958836513</v>
       </c>
       <c r="N19" s="0" t="s">
         <v>20</v>
@@ -1316,7 +1316,7 @@
         <v>2050</v>
       </c>
       <c r="P19" s="0" t="n">
-        <v>0.0662984958836513</v>
+        <v>0.0458851845244717</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,7 +1330,7 @@
         <v>10665</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0.0440974583945858</v>
+        <v>0.229414338428418</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>18</v>
@@ -1339,7 +1339,7 @@
         <v>9397</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>0.229414338428418</v>
+        <v>0.202138447089718</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>21</v>
@@ -1348,7 +1348,7 @@
         <v>2578</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0.202138447089718</v>
+        <v>0.0554552428006059</v>
       </c>
       <c r="K20" s="0" t="s">
         <v>20</v>
@@ -1357,7 +1357,7 @@
         <v>2280</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>0.0554552428006059</v>
+        <v>0.0490449781169052</v>
       </c>
       <c r="N20" s="0" t="s">
         <v>19</v>
@@ -1366,7 +1366,7 @@
         <v>2178</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>0.0490449781169052</v>
+        <v>0.0468508606748331</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,7 +1380,7 @@
         <v>3398</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0.162028013438356</v>
+        <v>0.252787506732569</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>17</v>
@@ -1389,7 +1389,7 @@
         <v>3009</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>0.252787506732569</v>
+        <v>0.223848619116627</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>19</v>
@@ -1398,7 +1398,7 @@
         <v>1025</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>0.223848619116627</v>
+        <v>0.0762528529725966</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>21</v>
@@ -1407,7 +1407,7 @@
         <v>802</v>
       </c>
       <c r="M21" s="0" t="n">
-        <v>0.0762528529725966</v>
+        <v>0.0596632078868512</v>
       </c>
       <c r="N21" s="0" t="s">
         <v>20</v>
@@ -1416,7 +1416,7 @@
         <v>616</v>
       </c>
       <c r="P21" s="0" t="n">
-        <v>0.0596632078868512</v>
+        <v>0.0458261048108483</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,7 +1430,7 @@
         <v>11481</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0.0101890936999643</v>
+        <v>0.189904196054042</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>18</v>
@@ -1439,7 +1439,7 @@
         <v>10568</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>0.189904196054042</v>
+        <v>0.174802503605881</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>20</v>
@@ -1448,7 +1448,7 @@
         <v>2540</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>0.174802503605881</v>
+        <v>0.0420134707758267</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>19</v>
@@ -1457,7 +1457,7 @@
         <v>2040</v>
       </c>
       <c r="M22" s="0" t="n">
-        <v>0.0420134707758267</v>
+        <v>0.0337431025128687</v>
       </c>
       <c r="N22" s="0" t="s">
         <v>21</v>
@@ -1466,7 +1466,7 @@
         <v>1903</v>
       </c>
       <c r="P22" s="0" t="n">
-        <v>0.0337431025128687</v>
+        <v>0.0314770216088182</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,7 +1480,7 @@
         <v>12750</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0.0276097086936342</v>
+        <v>0.184983597395605</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>17</v>
@@ -1489,7 +1489,7 @@
         <v>12130</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0.184983597395605</v>
+        <v>0.175988316581074</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>21</v>
@@ -1498,7 +1498,7 @@
         <v>3229</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>0.175988316581074</v>
+        <v>0.0468480028227772</v>
       </c>
       <c r="K23" s="0" t="s">
         <v>19</v>
@@ -1507,7 +1507,7 @@
         <v>2784</v>
       </c>
       <c r="M23" s="0" t="n">
-        <v>0.0468480028227772</v>
+        <v>0.0403917125607345</v>
       </c>
       <c r="N23" s="0" t="s">
         <v>20</v>
@@ -1516,7 +1516,7 @@
         <v>2475</v>
       </c>
       <c r="P23" s="0" t="n">
-        <v>0.0403917125607345</v>
+        <v>0.0359085806709116</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,7 +1530,7 @@
         <v>24794</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.02478257173403</v>
+        <v>0.24826629639335</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>18</v>
@@ -1539,7 +1539,7 @@
         <v>20732</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0.24826629639335</v>
+        <v>0.207592839268651</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>19</v>
@@ -1548,7 +1548,7 @@
         <v>5848</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>0.207592839268651</v>
+        <v>0.0585569614143869</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>20</v>
@@ -1557,7 +1557,7 @@
         <v>4666</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>0.0585569614143869</v>
+        <v>0.046721405943832</v>
       </c>
       <c r="N24" s="0" t="s">
         <v>21</v>
@@ -1566,7 +1566,7 @@
         <v>4647</v>
       </c>
       <c r="P24" s="0" t="n">
-        <v>0.046721405943832</v>
+        <v>0.046531155898197</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,7 +1580,7 @@
         <v>9925</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>0.0823989934094991</v>
+        <v>0.175986660122504</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>17</v>
@@ -1589,7 +1589,7 @@
         <v>7844</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0.175986660122504</v>
+        <v>0.13908708937037</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>21</v>
@@ -1598,7 +1598,7 @@
         <v>2574</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>0.13908708937037</v>
+        <v>0.0456412758846677</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>19</v>
@@ -1607,7 +1607,7 @@
         <v>2351</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>0.0456412758846677</v>
+        <v>0.0416871171736028</v>
       </c>
       <c r="N25" s="0" t="s">
         <v>20</v>
@@ -1616,7 +1616,7 @@
         <v>2238</v>
       </c>
       <c r="P25" s="0" t="n">
-        <v>0.0416871171736028</v>
+        <v>0.0396834403379511</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,7 +1630,7 @@
         <v>7969</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0.0751978479572091</v>
+        <v>0.267762131533065</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>18</v>
@@ -1639,7 +1639,7 @@
         <v>6485</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.267762131533065</v>
+        <v>0.217899036640975</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>19</v>
@@ -1648,7 +1648,7 @@
         <v>1924</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>0.217899036640975</v>
+        <v>0.0646473009247857</v>
       </c>
       <c r="K26" s="0" t="s">
         <v>21</v>
@@ -1657,7 +1657,7 @@
         <v>1814</v>
       </c>
       <c r="M26" s="0" t="n">
-        <v>0.0646473009247857</v>
+        <v>0.0609512494166119</v>
       </c>
       <c r="N26" s="0" t="s">
         <v>20</v>
@@ -1666,7 +1666,7 @@
         <v>1734</v>
       </c>
       <c r="P26" s="0" t="n">
-        <v>0.0609512494166119</v>
+        <v>0.0582632119561218</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,7 +1680,7 @@
         <v>14808</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0.0261681695757753</v>
+        <v>0.223470735339147</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>18</v>
@@ -1689,7 +1689,7 @@
         <v>12965</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.223470735339147</v>
+        <v>0.195657623154514</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>19</v>
@@ -1698,7 +1698,7 @@
         <v>3935</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>0.195657623154514</v>
+        <v>0.0593839373014279</v>
       </c>
       <c r="K27" s="0" t="s">
         <v>21</v>
@@ -1707,7 +1707,7 @@
         <v>3309</v>
       </c>
       <c r="M27" s="0" t="n">
-        <v>0.0593839373014279</v>
+        <v>0.0499368357129415</v>
       </c>
       <c r="N27" s="0" t="s">
         <v>20</v>
@@ -1716,7 +1716,7 @@
         <v>3037</v>
       </c>
       <c r="P27" s="0" t="n">
-        <v>0.0499368357129415</v>
+        <v>0.0458320247990944</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1730,7 +1730,7 @@
         <v>2130</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>0.284156298127394</v>
+        <v>0.199293024369888</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>17</v>
@@ -1739,7 +1739,7 @@
         <v>2104</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>0.199293024369888</v>
+        <v>0.196860339565373</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>19</v>
@@ -1748,7 +1748,7 @@
         <v>679</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>0.196860339565373</v>
+        <v>0.0635304993179126</v>
       </c>
       <c r="K28" s="0" t="s">
         <v>21</v>
@@ -1757,7 +1757,7 @@
         <v>637</v>
       </c>
       <c r="M28" s="0" t="n">
-        <v>0.0635304993179126</v>
+        <v>0.059600777710619</v>
       </c>
       <c r="N28" s="0" t="s">
         <v>20</v>
@@ -1766,7 +1766,7 @@
         <v>458</v>
       </c>
       <c r="P28" s="0" t="n">
-        <v>0.059600777710619</v>
+        <v>0.0428526784795346</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1780,7 @@
         <v>3591</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>0.0236764943073023</v>
+        <v>0.185638190081927</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>18</v>
@@ -1789,7 +1789,7 @@
         <v>3514</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>0.185638190081927</v>
+        <v>0.181657644095765</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>19</v>
@@ -1798,7 +1798,7 @@
         <v>1174</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>0.181657644095765</v>
+        <v>0.0606904024383687</v>
       </c>
       <c r="K29" s="0" t="s">
         <v>21</v>
@@ -1807,7 +1807,7 @@
         <v>799</v>
       </c>
       <c r="M29" s="0" t="n">
-        <v>0.0606904024383687</v>
+        <v>0.0413046265317348</v>
       </c>
       <c r="N29" s="0" t="s">
         <v>20</v>
@@ -1816,7 +1816,7 @@
         <v>776</v>
       </c>
       <c r="P29" s="0" t="n">
-        <v>0.0413046265317348</v>
+        <v>0.0401156322761279</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,7 +1830,7 @@
         <v>6114</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.0251935291589127</v>
+        <v>0.198496439790712</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>18</v>
@@ -1839,7 +1839,7 @@
         <v>5015</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.198496439790712</v>
+        <v>0.162816428778283</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>19</v>
@@ -1848,7 +1848,7 @@
         <v>1617</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>0.162816428778283</v>
+        <v>0.0524973410437653</v>
       </c>
       <c r="K30" s="0" t="s">
         <v>21</v>
@@ -1857,7 +1857,7 @@
         <v>1340</v>
       </c>
       <c r="M30" s="0" t="n">
-        <v>0.0524973410437653</v>
+        <v>0.0435042900424524</v>
       </c>
       <c r="N30" s="0" t="s">
         <v>20</v>
@@ -1866,7 +1866,7 @@
         <v>1078</v>
       </c>
       <c r="P30" s="0" t="n">
-        <v>0.0435042900424524</v>
+        <v>0.0349982273625102</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,7 +1880,7 @@
         <v>2773</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0.0792815532124106</v>
+        <v>0.203940396157713</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>17</v>
@@ -1889,7 +1889,7 @@
         <v>2571</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>0.203940396157713</v>
+        <v>0.189084298060397</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>21</v>
@@ -1898,7 +1898,7 @@
         <v>815</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>0.189084298060397</v>
+        <v>0.0599392076698651</v>
       </c>
       <c r="K31" s="0" t="s">
         <v>19</v>
@@ -1907,7 +1907,7 @@
         <v>705</v>
       </c>
       <c r="M31" s="0" t="n">
-        <v>0.0599392076698651</v>
+        <v>0.0518492532604355</v>
       </c>
       <c r="N31" s="0" t="s">
         <v>20</v>
@@ -1916,7 +1916,7 @@
         <v>457</v>
       </c>
       <c r="P31" s="0" t="n">
-        <v>0.0518492532604355</v>
+        <v>0.0336100833191759</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +1930,7 @@
         <v>18647</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0.00514512749670971</v>
+        <v>0.209936963744302</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>18</v>
@@ -1939,7 +1939,7 @@
         <v>16270</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>0.209936963744302</v>
+        <v>0.183175545670606</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>20</v>
@@ -1948,7 +1948,7 @@
         <v>3413</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>0.183175545670606</v>
+        <v>0.0384252081975279</v>
       </c>
       <c r="K32" s="0" t="s">
         <v>21</v>
@@ -1957,7 +1957,7 @@
         <v>3218</v>
       </c>
       <c r="M32" s="0" t="n">
-        <v>0.0384252081975279</v>
+        <v>0.0362298036858027</v>
       </c>
       <c r="N32" s="0" t="s">
         <v>19</v>
@@ -1966,7 +1966,7 @@
         <v>3202</v>
       </c>
       <c r="P32" s="0" t="n">
-        <v>0.0362298036858027</v>
+        <v>0.0360496679309945</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,7 +1980,7 @@
         <v>3591</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0.152706777710533</v>
+        <v>0.171258600486735</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>17</v>
@@ -1989,7 +1989,7 @@
         <v>3508</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>0.171258600486735</v>
+        <v>0.167300242413664</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>21</v>
@@ -1998,7 +1998,7 @@
         <v>1430</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>0.167300242413664</v>
+        <v>0.0681982174035174</v>
       </c>
       <c r="K33" s="0" t="s">
         <v>19</v>
@@ -2007,7 +2007,7 @@
         <v>1109</v>
       </c>
       <c r="M33" s="0" t="n">
-        <v>0.0681982174035174</v>
+        <v>0.052889386783567</v>
       </c>
       <c r="N33" s="0" t="s">
         <v>20</v>
@@ -2016,7 +2016,7 @@
         <v>786</v>
       </c>
       <c r="P33" s="0" t="n">
-        <v>0.052889386783567</v>
+        <v>0.0374851740413739</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2030,7 +2030,7 @@
         <v>44450</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>0.00404039137101942</v>
+        <v>0.228492870791111</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>18</v>
@@ -2039,7 +2039,7 @@
         <v>35089</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>0.228492870791111</v>
+        <v>0.180373146078499</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>19</v>
@@ -2048,7 +2048,7 @@
         <v>7109</v>
       </c>
       <c r="J34" s="0" t="n">
-        <v>0.180373146078499</v>
+        <v>0.036543437985467</v>
       </c>
       <c r="K34" s="0" t="s">
         <v>21</v>
@@ -2057,7 +2057,7 @@
         <v>6515</v>
       </c>
       <c r="M34" s="0" t="n">
-        <v>0.036543437985467</v>
+        <v>0.0334900124455363</v>
       </c>
       <c r="N34" s="0" t="s">
         <v>20</v>
@@ -2066,7 +2066,7 @@
         <v>6292</v>
       </c>
       <c r="P34" s="0" t="n">
-        <v>0.0334900124455363</v>
+        <v>0.0323436927563031</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,7 +2080,7 @@
         <v>19322</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>0.0599918917506763</v>
+        <v>0.184228120217191</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>17</v>
@@ -2089,7 +2089,7 @@
         <v>18474</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>0.184228120217191</v>
+        <v>0.176142754005403</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>19</v>
@@ -2098,7 +2098,7 @@
         <v>5221</v>
       </c>
       <c r="J35" s="0" t="n">
-        <v>0.176142754005403</v>
+        <v>0.0497803030563066</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>20</v>
@@ -2107,7 +2107,7 @@
         <v>5033</v>
       </c>
       <c r="M35" s="0" t="n">
-        <v>0.0497803030563066</v>
+        <v>0.047987792622561</v>
       </c>
       <c r="N35" s="0" t="s">
         <v>21</v>
@@ -2116,7 +2116,7 @@
         <v>4991</v>
       </c>
       <c r="P35" s="0" t="n">
-        <v>0.047987792622561</v>
+        <v>0.0475873381639583</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2130,7 @@
         <v>1323</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>0.65493358808076</v>
+        <v>0.173607921665166</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>18</v>
@@ -2139,7 +2139,7 @@
         <v>1320</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>0.173607921665166</v>
+        <v>0.173214252908556</v>
       </c>
       <c r="H36" s="0" t="s">
         <v>25</v>
@@ -2148,7 +2148,7 @@
         <v>376</v>
       </c>
       <c r="J36" s="0" t="n">
-        <v>0.173214252908556</v>
+        <v>0.0493398174951644</v>
       </c>
       <c r="K36" s="0" t="s">
         <v>21</v>
@@ -2157,7 +2157,7 @@
         <v>368</v>
       </c>
       <c r="M36" s="0" t="n">
-        <v>0.0493398174951644</v>
+        <v>0.0482900341442035</v>
       </c>
       <c r="N36" s="0" t="s">
         <v>19</v>
@@ -2166,7 +2166,7 @@
         <v>351</v>
       </c>
       <c r="P36" s="0" t="n">
-        <v>0.0482900341442035</v>
+        <v>0.0460592445234115</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,7 +2180,7 @@
         <v>28069</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0.00300279747799232</v>
+        <v>0.240129693475118</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>18</v>
@@ -2189,7 +2189,7 @@
         <v>25396</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>0.240129693475118</v>
+        <v>0.217262235758099</v>
       </c>
       <c r="H37" s="0" t="s">
         <v>19</v>
@@ -2198,7 +2198,7 @@
         <v>7211</v>
       </c>
       <c r="J37" s="0" t="n">
-        <v>0.217262235758099</v>
+        <v>0.0616899504666741</v>
       </c>
       <c r="K37" s="0" t="s">
         <v>21</v>
@@ -2207,7 +2207,7 @@
         <v>6756</v>
       </c>
       <c r="M37" s="0" t="n">
-        <v>0.0616899504666741</v>
+        <v>0.0577974352174248</v>
       </c>
       <c r="N37" s="0" t="s">
         <v>20</v>
@@ -2216,7 +2216,7 @@
         <v>5945</v>
       </c>
       <c r="P37" s="0" t="n">
-        <v>0.0577974352174248</v>
+        <v>0.0508593475973343</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2230,7 +2230,7 @@
         <v>10310</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0.150241181954581</v>
+        <v>0.26055283195151</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>18</v>
@@ -2239,7 +2239,7 @@
         <v>8280</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>0.26055283195151</v>
+        <v>0.209250964942629</v>
       </c>
       <c r="H38" s="0" t="s">
         <v>19</v>
@@ -2248,7 +2248,7 @@
         <v>2924</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>0.209250964942629</v>
+        <v>0.0738949059773246</v>
       </c>
       <c r="K38" s="0" t="s">
         <v>21</v>
@@ -2257,7 +2257,7 @@
         <v>2422</v>
       </c>
       <c r="M38" s="0" t="n">
-        <v>0.0738949059773246</v>
+        <v>0.061208434431286</v>
       </c>
       <c r="N38" s="0" t="s">
         <v>20</v>
@@ -2266,7 +2266,7 @@
         <v>1881</v>
       </c>
       <c r="P38" s="0" t="n">
-        <v>0.061208434431286</v>
+        <v>0.0475363605141407</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,7 +2280,7 @@
         <v>8093</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.0445973753223589</v>
+        <v>0.191880148050957</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>17</v>
@@ -2289,7 +2289,7 @@
         <v>6859</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>0.191880148050957</v>
+        <v>0.162622752438097</v>
       </c>
       <c r="H39" s="0" t="s">
         <v>19</v>
@@ -2298,7 +2298,7 @@
         <v>2119</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>0.162622752438097</v>
+        <v>0.0502402117533644</v>
       </c>
       <c r="K39" s="0" t="s">
         <v>21</v>
@@ -2307,7 +2307,7 @@
         <v>1999</v>
       </c>
       <c r="M39" s="0" t="n">
-        <v>0.0502402117533644</v>
+        <v>0.0473950841410927</v>
       </c>
       <c r="N39" s="0" t="s">
         <v>20</v>
@@ -2316,7 +2316,7 @@
         <v>1873</v>
       </c>
       <c r="P39" s="0" t="n">
-        <v>0.0473950841410927</v>
+        <v>0.0444077001482074</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2330,7 @@
         <v>32042</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>0.0146305390513927</v>
+        <v>0.250289232399747</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>18</v>
@@ -2339,7 +2339,7 @@
         <v>28697</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>0.250289232399747</v>
+        <v>0.224160480062903</v>
       </c>
       <c r="H40" s="0" t="s">
         <v>21</v>
@@ -2348,7 +2348,7 @@
         <v>7324</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>0.224160480062903</v>
+        <v>0.0572098601240792</v>
       </c>
       <c r="K40" s="0" t="s">
         <v>20</v>
@@ -2357,7 +2357,7 @@
         <v>6987</v>
       </c>
       <c r="M40" s="0" t="n">
-        <v>0.0572098601240792</v>
+        <v>0.0545774566748964</v>
       </c>
       <c r="N40" s="0" t="s">
         <v>19</v>
@@ -2366,7 +2366,7 @@
         <v>6664</v>
       </c>
       <c r="P40" s="0" t="n">
-        <v>0.0545774566748964</v>
+        <v>0.0520544112325046</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2380,7 +2380,7 @@
         <v>2371</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>0.629058460713581</v>
+        <v>0.223814167219673</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>18</v>
@@ -2389,7 +2389,7 @@
         <v>2226</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>0.223814167219673</v>
+        <v>0.210126670700545</v>
       </c>
       <c r="H41" s="0" t="s">
         <v>21</v>
@@ -2398,7 +2398,7 @@
         <v>649</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>0.210126670700545</v>
+        <v>0.0612633464890627</v>
       </c>
       <c r="K41" s="0" t="s">
         <v>19</v>
@@ -2407,7 +2407,7 @@
         <v>510</v>
       </c>
       <c r="M41" s="0" t="n">
-        <v>0.0612633464890627</v>
+        <v>0.0481422291362435</v>
       </c>
       <c r="N41" s="0" t="s">
         <v>25</v>
@@ -2416,7 +2416,7 @@
         <v>453</v>
       </c>
       <c r="P41" s="0" t="n">
-        <v>0.0481422291362435</v>
+        <v>0.0427616270563104</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2430,7 @@
         <v>10092</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>0.00879831352061894</v>
+        <v>0.196010110485842</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>18</v>
@@ -2439,7 +2439,7 @@
         <v>9950</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>0.196010110485842</v>
+        <v>0.193252140243175</v>
       </c>
       <c r="H42" s="0" t="s">
         <v>19</v>
@@ -2448,7 +2448,7 @@
         <v>2908</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>0.193252140243175</v>
+        <v>0.0564801229977039</v>
       </c>
       <c r="K42" s="0" t="s">
         <v>21</v>
@@ -2457,7 +2457,7 @@
         <v>2737</v>
       </c>
       <c r="M42" s="0" t="n">
-        <v>0.0564801229977039</v>
+        <v>0.0531589053111126</v>
       </c>
       <c r="N42" s="0" t="s">
         <v>20</v>
@@ -2466,7 +2466,7 @@
         <v>2600</v>
       </c>
       <c r="P42" s="0" t="n">
-        <v>0.0531589053111126</v>
+        <v>0.0504980466967091</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,7 +2480,7 @@
         <v>1711</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>0.293898553001778</v>
+        <v>0.19340785545617</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>18</v>
@@ -2489,7 +2489,7 @@
         <v>1640</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>0.19340785545617</v>
+        <v>0.185382164201122</v>
       </c>
       <c r="H43" s="0" t="s">
         <v>19</v>
@@ -2498,7 +2498,7 @@
         <v>502</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>0.185382164201122</v>
+        <v>0.0567450283103433</v>
       </c>
       <c r="K43" s="0" t="s">
         <v>21</v>
@@ -2507,7 +2507,7 @@
         <v>469</v>
       </c>
       <c r="M43" s="0" t="n">
-        <v>0.0567450283103433</v>
+        <v>0.0530147774453207</v>
       </c>
       <c r="N43" s="0" t="s">
         <v>25</v>
@@ -2516,7 +2516,7 @@
         <v>421</v>
       </c>
       <c r="P43" s="0" t="n">
-        <v>0.0530147774453207</v>
+        <v>0.0475889580052879</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2530,7 +2530,7 @@
         <v>15730</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>0.00616472797442268</v>
+        <v>0.230335323129854</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>18</v>
@@ -2539,7 +2539,7 @@
         <v>14214</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>0.230335323129854</v>
+        <v>0.208136445198204</v>
       </c>
       <c r="H44" s="0" t="s">
         <v>19</v>
@@ -2548,7 +2548,7 @@
         <v>4239</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>0.208136445198204</v>
+        <v>0.0620719284645552</v>
       </c>
       <c r="K44" s="0" t="s">
         <v>21</v>
@@ -2557,7 +2557,7 @@
         <v>3873</v>
       </c>
       <c r="M44" s="0" t="n">
-        <v>0.0620719284645552</v>
+        <v>0.0567125687528243</v>
       </c>
       <c r="N44" s="0" t="s">
         <v>20</v>
@@ -2566,7 +2566,7 @@
         <v>3447</v>
       </c>
       <c r="P44" s="0" t="n">
-        <v>0.0567125687528243</v>
+        <v>0.0504746254817933</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,7 +2580,7 @@
         <v>43298</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>0.0118878953876242</v>
+        <v>0.149324657526357</v>
       </c>
       <c r="E45" s="0" t="s">
         <v>18</v>
@@ -2589,7 +2589,7 @@
         <v>39121</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>0.149324657526357</v>
+        <v>0.134919163173556</v>
       </c>
       <c r="H45" s="0" t="s">
         <v>20</v>
@@ -2598,7 +2598,7 @@
         <v>10485</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>0.134919163173556</v>
+        <v>0.0361603084244966</v>
       </c>
       <c r="K45" s="0" t="s">
         <v>19</v>
@@ -2607,7 +2607,7 @@
         <v>10231</v>
       </c>
       <c r="M45" s="0" t="n">
-        <v>0.0361603084244966</v>
+        <v>0.0352843219352431</v>
       </c>
       <c r="N45" s="0" t="s">
         <v>21</v>
@@ -2616,7 +2616,7 @@
         <v>9976</v>
       </c>
       <c r="P45" s="0" t="n">
-        <v>0.0352843219352431</v>
+        <v>0.034404886680284</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,7 +2630,7 @@
         <v>3598</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>0.311170639166202</v>
+        <v>0.112228544478749</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>18</v>
@@ -2639,7 +2639,7 @@
         <v>3091</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>0.112228544478749</v>
+        <v>0.0964142387392474</v>
       </c>
       <c r="H46" s="0" t="s">
         <v>21</v>
@@ -2648,7 +2648,7 @@
         <v>1223</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>0.0964142387392474</v>
+        <v>0.0381477237069232</v>
       </c>
       <c r="K46" s="0" t="s">
         <v>25</v>
@@ -2657,7 +2657,7 @@
         <v>906</v>
       </c>
       <c r="M46" s="0" t="n">
-        <v>0.0381477237069232</v>
+        <v>0.0282598836291679</v>
       </c>
       <c r="N46" s="0" t="s">
         <v>20</v>
@@ -2666,7 +2666,7 @@
         <v>888</v>
       </c>
       <c r="P46" s="0" t="n">
-        <v>0.0282598836291679</v>
+        <v>0.0276984289875288</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2680,7 +2680,7 @@
         <v>1399</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>0.142310200981107</v>
+        <v>0.224202670239379</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>17</v>
@@ -2689,7 +2689,7 @@
         <v>1311</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>0.224202670239379</v>
+        <v>0.21009985752954</v>
       </c>
       <c r="H47" s="0" t="s">
         <v>19</v>
@@ -2698,7 +2698,7 @@
         <v>357</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>0.21009985752954</v>
+        <v>0.0572125470160532</v>
       </c>
       <c r="K47" s="0" t="s">
         <v>21</v>
@@ -2707,7 +2707,7 @@
         <v>346</v>
       </c>
       <c r="M47" s="0" t="n">
-        <v>0.0572125470160532</v>
+        <v>0.0554496954273232</v>
       </c>
       <c r="N47" s="0" t="s">
         <v>20</v>
@@ -2716,7 +2716,7 @@
         <v>307</v>
       </c>
       <c r="P47" s="0" t="n">
-        <v>0.0554496954273232</v>
+        <v>0.0491995852490989</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,7 +2730,7 @@
         <v>14947</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>0.00359673500814655</v>
+        <v>0.175115303474809</v>
       </c>
       <c r="E48" s="0" t="s">
         <v>17</v>
@@ -2739,7 +2739,7 @@
         <v>14077</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>0.175115303474809</v>
+        <v>0.164922601660192</v>
       </c>
       <c r="H48" s="0" t="s">
         <v>21</v>
@@ -2748,7 +2748,7 @@
         <v>3429</v>
       </c>
       <c r="J48" s="0" t="n">
-        <v>0.164922601660192</v>
+        <v>0.0401733040486466</v>
       </c>
       <c r="K48" s="0" t="s">
         <v>20</v>
@@ -2757,7 +2757,7 @@
         <v>3393</v>
       </c>
       <c r="M48" s="0" t="n">
-        <v>0.0401733040486466</v>
+        <v>0.0397515370770073</v>
       </c>
       <c r="N48" s="0" t="s">
         <v>19</v>
@@ -2766,7 +2766,7 @@
         <v>3370</v>
       </c>
       <c r="P48" s="0" t="n">
-        <v>0.0397515370770073</v>
+        <v>0.0394820748451266</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2780,7 +2780,7 @@
         <v>12687</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>0.0442553821833084</v>
+        <v>0.166607725151227</v>
       </c>
       <c r="E49" s="0" t="s">
         <v>17</v>
@@ -2789,7 +2789,7 @@
         <v>11025</v>
       </c>
       <c r="G49" s="0" t="n">
-        <v>0.166607725151227</v>
+        <v>0.144782073759933</v>
       </c>
       <c r="H49" s="0" t="s">
         <v>25</v>
@@ -2798,7 +2798,7 @@
         <v>3490</v>
       </c>
       <c r="J49" s="0" t="n">
-        <v>0.144782073759933</v>
+        <v>0.045831241489539</v>
       </c>
       <c r="K49" s="0" t="s">
         <v>21</v>
@@ -2807,7 +2807,7 @@
         <v>3192</v>
       </c>
       <c r="M49" s="0" t="n">
-        <v>0.045831241489539</v>
+        <v>0.0419178575457331</v>
       </c>
       <c r="N49" s="0" t="s">
         <v>19</v>
@@ -2816,7 +2816,7 @@
         <v>3154</v>
       </c>
       <c r="P49" s="0" t="n">
-        <v>0.0419178575457331</v>
+        <v>0.0414188354320934</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2830,7 @@
         <v>4839</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>0.175990027603762</v>
+        <v>0.270011332775715</v>
       </c>
       <c r="E50" s="0" t="s">
         <v>17</v>
@@ -2839,7 +2839,7 @@
         <v>4727</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>0.270011332775715</v>
+        <v>0.263761845428974</v>
       </c>
       <c r="H50" s="0" t="s">
         <v>19</v>
@@ -2848,7 +2848,7 @@
         <v>1628</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>0.263761845428974</v>
+        <v>0.0908407625044151</v>
       </c>
       <c r="K50" s="0" t="s">
         <v>21</v>
@@ -2857,7 +2857,7 @@
         <v>1516</v>
       </c>
       <c r="M50" s="0" t="n">
-        <v>0.0908407625044151</v>
+        <v>0.084591275157674</v>
       </c>
       <c r="N50" s="0" t="s">
         <v>20</v>
@@ -2866,7 +2866,7 @@
         <v>1079</v>
       </c>
       <c r="P50" s="0" t="n">
-        <v>0.084591275157674</v>
+        <v>0.0602071147065503</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,7 +2880,7 @@
         <v>11473</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>0.0185317686726891</v>
+        <v>0.197048176072069</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>18</v>
@@ -2889,7 +2889,7 @@
         <v>11423</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>0.197048176072069</v>
+        <v>0.196189428682232</v>
       </c>
       <c r="H51" s="0" t="s">
         <v>21</v>
@@ -2898,7 +2898,7 @@
         <v>3206</v>
       </c>
       <c r="J51" s="0" t="n">
-        <v>0.196189428682232</v>
+        <v>0.0550628826363682</v>
       </c>
       <c r="K51" s="0" t="s">
         <v>19</v>
@@ -2907,7 +2907,7 @@
         <v>2846</v>
       </c>
       <c r="M51" s="0" t="n">
-        <v>0.0550628826363682</v>
+        <v>0.0488799014295396</v>
       </c>
       <c r="N51" s="0" t="s">
         <v>20</v>
@@ -2916,7 +2916,7 @@
         <v>2618</v>
       </c>
       <c r="P51" s="0" t="n">
-        <v>0.0488799014295396</v>
+        <v>0.0449640133318815</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,7 +2930,7 @@
         <v>1030</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0.452347177322512</v>
+        <v>0.177966994897704</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>18</v>
@@ -2939,7 +2939,7 @@
         <v>931</v>
       </c>
       <c r="G52" s="0" t="n">
-        <v>0.177966994897704</v>
+        <v>0.160861429368701</v>
       </c>
       <c r="H52" s="0" t="s">
         <v>21</v>
@@ -2948,7 +2948,7 @@
         <v>400</v>
       </c>
       <c r="J52" s="0" t="n">
-        <v>0.160861429368701</v>
+        <v>0.0691133960767781</v>
       </c>
       <c r="K52" s="0" t="s">
         <v>19</v>
@@ -2957,7 +2957,7 @@
         <v>368</v>
       </c>
       <c r="M52" s="0" t="n">
-        <v>0.0691133960767781</v>
+        <v>0.0635843243906358</v>
       </c>
       <c r="N52" s="0" t="s">
         <v>20</v>
@@ -2966,7 +2966,7 @@
         <v>198</v>
       </c>
       <c r="P52" s="0" t="n">
-        <v>0.0635843243906358</v>
+        <v>0.0342111310580051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>